<commit_message>
corrected roster and payments sheet
</commit_message>
<xml_diff>
--- a/section_2/JonathanSanchez_Week2Homework.xlsx
+++ b/section_2/JonathanSanchez_Week2Homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan.sanchez/Desktop/Homework/section_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFB19BF1-AA13-9140-AA1B-0A285FD7438F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B86AA5-0FB5-2041-B735-F352361F07B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23800" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="-23460" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="94" r:id="rId5"/>
-    <pivotCache cacheId="95" r:id="rId6"/>
+    <pivotCache cacheId="98" r:id="rId5"/>
+    <pivotCache cacheId="99" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="171">
   <si>
     <t>Expenses</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>Sum of Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -728,7 +731,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -755,6 +757,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1054,6 +1060,36 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total of Tax Inclusive</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Payments by Supplier </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4550,16 +4586,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7658,7 +7694,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A7EE90A-062E-944E-B05B-B96FD5D1807B}" name="PivotTable22" cacheId="95" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A7EE90A-062E-944E-B05B-B96FD5D1807B}" name="PivotTable22" cacheId="99" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="F11:G27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7878,7 +7914,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BA485541-5C40-CB4E-A345-F2E8489F8889}" name="PivotTable21" cacheId="94" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BA485541-5C40-CB4E-A345-F2E8489F8889}" name="PivotTable21" cacheId="98" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E46" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -8633,7 +8669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -8659,31 +8695,31 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -14721,1144 +14757,712 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC2E761-9565-2242-B46C-BFFD4ABE5101}">
-  <dimension ref="A3:G46"/>
+  <dimension ref="A3:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="19" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="19" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="19" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="19" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="19" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="19" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="19" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="19" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="19" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="19" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="19" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="19" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="19" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="19" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="19" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="19" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="19" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="19" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="19" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="19" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="19" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="19" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="19" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="19" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="19" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="19" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="19" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="19" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="19" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="19" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="19" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="19" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="19" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="19" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="19" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="19" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="19" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="19" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="19" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="19" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="19" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="19" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="19" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="19" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="19" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="19" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="19" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="19" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="19" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="19" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="19" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="19" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="19" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="19" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="19" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="19" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="19" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="19" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="19" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="19" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="19" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="19" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="19" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="19" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="19" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="19" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="19" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="19" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="19" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="19" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="19" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="19" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="19" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="19" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="19" bestFit="1" customWidth="1"/>
-    <col min="221" max="222" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="227" max="234" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="237" max="242" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="245" max="246" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="249" max="250" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="257" max="258" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="261" max="266" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="269" max="270" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="273" max="276" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="279" max="280" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="283" max="284" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="287" max="288" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="289" max="289" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="291" max="298" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="299" max="299" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="300" max="300" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="301" max="308" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="310" max="310" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="311" max="312" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="315" max="316" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="319" max="320" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="323" max="326" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="328" max="328" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="329" max="332" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="333" max="333" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="334" max="334" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="335" max="338" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="339" max="339" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="340" max="340" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="341" max="342" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="344" max="344" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="345" max="354" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="355" max="355" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="356" max="356" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="357" max="360" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="361" max="361" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="362" max="362" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="363" max="364" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="365" max="365" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="366" max="366" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="367" max="368" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="369" max="369" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="370" max="370" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="371" max="372" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="373" max="373" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="374" max="374" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="375" max="376" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="377" max="377" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="378" max="378" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="379" max="380" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="381" max="381" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="382" max="382" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="383" max="386" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="387" max="387" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="388" max="388" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="389" max="392" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="393" max="393" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="394" max="394" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="395" max="396" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="397" max="397" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="398" max="398" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="399" max="400" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="401" max="401" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="402" max="402" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="403" max="410" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="411" max="411" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="412" max="412" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="413" max="414" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="415" max="415" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="416" max="416" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="417" max="422" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="423" max="423" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="424" max="424" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="425" max="426" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="427" max="427" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="428" max="428" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="429" max="430" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="431" max="431" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="432" max="432" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="433" max="434" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="435" max="435" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="436" max="436" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="437" max="440" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="441" max="441" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="442" max="442" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="443" max="444" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="445" max="445" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="446" max="446" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="447" max="450" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="451" max="451" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="452" max="452" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="453" max="454" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="455" max="455" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="456" max="456" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="457" max="464" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="465" max="465" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="466" max="466" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="467" max="470" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="471" max="471" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="472" max="472" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="473" max="474" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="475" max="475" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="476" max="476" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="477" max="478" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="479" max="479" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="480" max="480" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="481" max="484" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="485" max="485" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="486" max="486" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="487" max="488" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="489" max="489" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="490" max="490" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="491" max="494" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="495" max="495" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="496" max="496" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="497" max="500" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="501" max="501" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="502" max="502" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="503" max="504" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="505" max="505" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="506" max="506" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="507" max="514" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="517" max="522" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="523" max="523" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="524" max="524" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="525" max="526" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="528" max="528" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="529" max="530" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="531" max="531" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="532" max="532" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="533" max="536" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="537" max="537" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="538" max="538" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="539" max="546" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="547" max="547" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="548" max="548" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="549" max="552" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="553" max="553" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="554" max="554" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="555" max="556" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="557" max="557" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="558" max="558" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="559" max="566" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="567" max="567" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="568" max="568" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="569" max="576" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="577" max="577" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="578" max="578" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="579" max="580" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="581" max="581" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="582" max="582" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="583" max="584" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="585" max="585" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="586" max="586" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="587" max="590" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="591" max="591" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="592" max="592" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="593" max="596" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="597" max="597" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="598" max="598" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="599" max="602" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="603" max="603" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="604" max="604" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="605" max="612" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="613" max="613" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="614" max="614" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="615" max="616" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="617" max="617" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="618" max="618" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="619" max="624" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="625" max="625" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="626" max="626" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="627" max="636" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="637" max="637" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="638" max="638" width="29" bestFit="1" customWidth="1"/>
-    <col min="639" max="639" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="640" max="640" width="27.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="I3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="I4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>160</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>70</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30">
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
         <v>40923</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>80</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>35</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
         <v>40954</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>80</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>35</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <v>680</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30">
         <v>680</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="28">
         <v>40913</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="30">
         <v>340</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30">
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="28">
         <v>40944</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
         <v>340</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30">
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>40240</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>0</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>-240</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>40000</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="31" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="28">
         <v>40928</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>20000</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>-20000</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30">
         <v>0</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="28">
         <v>40934</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30">
         <v>20000</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30">
         <v>20000</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="31">
         <v>680</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="29">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="28">
         <v>40939</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="30">
         <v>170</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30">
         <v>-170</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <v>0</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>40000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="29">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="28">
         <v>40959</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <v>20000</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>-20000</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30">
         <v>0</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="29">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="28">
         <v>40965</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30">
         <v>20000</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30">
         <v>20000</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="31">
         <v>64965.25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="29">
+      <c r="A17" s="28">
         <v>40968</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
         <v>70</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30">
         <v>-70</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="30">
         <v>0</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="31">
         <v>640</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30">
         <v>61</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="30">
         <v>61</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <v>2000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="29">
+      <c r="A19" s="28">
         <v>40929</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31">
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30">
         <v>61</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="30">
         <v>61</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>5900</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="30">
         <v>640</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30">
         <v>640</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="29">
+      <c r="A21" s="28">
         <v>40934</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="30">
         <v>320</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30">
         <v>320</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="29">
+      <c r="A22" s="28">
         <v>40965</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="30">
         <v>320</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30">
         <v>320</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="30">
         <v>2000</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31">
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30">
         <v>2000</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="31">
         <v>12800</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
+      <c r="A24" s="28">
         <v>40910</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="30">
         <v>1000</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31">
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30">
         <v>1000</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="31">
         <v>389.25</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="29">
+      <c r="A25" s="28">
         <v>40941</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="30">
         <v>1000</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31">
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30">
         <v>1000</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="31">
         <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="30">
         <v>5900</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30">
         <v>5900</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="31">
         <v>1476</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
+      <c r="A27" s="28">
         <v>40964</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="30">
         <v>2200</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30">
         <v>2200</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="31">
         <v>129930.5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="29">
+      <c r="A28" s="28">
         <v>40968</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="30">
         <v>3700</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31">
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30">
         <v>3700</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30">
         <v>180</v>
       </c>
-      <c r="E29" s="31">
+      <c r="E29" s="30">
         <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="29">
+      <c r="A30" s="28">
         <v>40924</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31">
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30">
         <v>105</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="30">
         <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="29">
+      <c r="A31" s="28">
         <v>40964</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31">
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30">
         <v>75</v>
       </c>
-      <c r="E31" s="31">
+      <c r="E31" s="30">
         <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="31">
+      <c r="B32" s="30">
         <v>179</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31">
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30">
         <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="29">
+      <c r="A33" s="28">
         <v>40939</v>
       </c>
-      <c r="B33" s="31">
+      <c r="B33" s="30">
         <v>179</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30">
         <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="31">
+      <c r="B34" s="30">
         <v>120</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30">
         <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="29">
+      <c r="A35" s="28">
         <v>40924</v>
       </c>
-      <c r="B35" s="31">
+      <c r="B35" s="30">
         <v>120</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31">
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="31">
+      <c r="B36" s="30">
         <v>12800</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31">
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30">
         <v>12800</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="29">
+      <c r="A37" s="28">
         <v>40934</v>
       </c>
-      <c r="B37" s="31">
+      <c r="B37" s="30">
         <v>6400</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31">
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30">
         <v>6400</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="29">
+      <c r="A38" s="28">
         <v>40965</v>
       </c>
-      <c r="B38" s="31">
+      <c r="B38" s="30">
         <v>6400</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31">
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30">
         <v>6400</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="31">
+      <c r="B39" s="30">
         <v>389.25</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30">
         <v>389.25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="29">
+      <c r="A40" s="28">
         <v>40939</v>
       </c>
-      <c r="B40" s="31">
+      <c r="B40" s="30">
         <v>389.25</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31">
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30">
         <v>389.25</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="31">
+      <c r="B41" s="30">
         <v>310</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31">
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30">
         <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="29">
+      <c r="A42" s="28">
         <v>40924</v>
       </c>
-      <c r="B42" s="31">
+      <c r="B42" s="30">
         <v>310</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31">
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30">
         <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="31">
+      <c r="B43" s="30">
         <v>1476</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31">
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30">
         <v>1476</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="29">
+      <c r="A44" s="28">
         <v>40924</v>
       </c>
-      <c r="B44" s="31">
+      <c r="B44" s="30">
         <v>962</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31">
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30">
         <v>962</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="29">
+      <c r="A45" s="28">
         <v>40966</v>
       </c>
-      <c r="B45" s="31">
+      <c r="B45" s="30">
         <v>514</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30">
         <v>514</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="31">
+      <c r="B46" s="30">
         <v>64894.25</v>
       </c>
-      <c r="C46" s="31">
+      <c r="C46" s="30">
         <v>70</v>
       </c>
-      <c r="D46" s="31">
+      <c r="D46" s="30">
         <v>1</v>
       </c>
-      <c r="E46" s="31">
+      <c r="E46" s="30">
         <v>64965.25</v>
       </c>
     </row>
@@ -15870,23 +15474,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A80E064-74CB-D24C-BB34-483708FB3A0C}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" ht="44" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>144</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -16068,57 +15665,107 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="20">
-        <f>MIN(C4:D14)</f>
+      <c r="B24" s="32">
+        <f>MIN(C4:C14)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="E24" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" s="32">
+        <f>MIN(D4:D14)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="20">
-        <f>MAX(C4:D14)</f>
+      <c r="B25" s="32">
+        <f>MAX(C4:C14)</f>
+        <v>15</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="32">
+        <f>MAX(D4:D14)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="20">
-        <f>AVERAGE(C4:D14)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="B26" s="32">
+        <f>AVERAGE(C4:C14)</f>
+        <v>12.454545454545455</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="32">
+        <f>AVERAGE(D4:D14)</f>
+        <v>83.545454545454547</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="20">
-        <f>MODE(C4:D14)</f>
+      <c r="B27" s="32">
+        <f>MODE(C4:C14)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="E27" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" s="32">
+        <f>MODE(D4:D14)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="20">
-        <f>MEDIAN(C4:D14)</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+      <c r="B28" s="32">
+        <f>MEDIAN(C4:C14)</f>
+        <v>12</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" s="32">
+        <f>MEDIAN(D4:D14)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B29" s="32">
         <f>COUNT(C4:C14)</f>
+        <v>11</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" s="32">
+        <f>COUNT(D4:D14)</f>
         <v>11</v>
       </c>
     </row>

</xml_diff>